<commit_message>
V8.0 beta, going for an optimized BOM
V8.0 beta, going for an optimized BOM resulting in 2,5 EUR cheaper in raw component cost.
</commit_message>
<xml_diff>
--- a/V8.0 - Beta/Price estemate.xlsx
+++ b/V8.0 - Beta/Price estemate.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="175">
   <si>
     <t>Ref-Des</t>
   </si>
@@ -555,6 +555,9 @@
   </si>
   <si>
     <t>Price komp pr:</t>
+  </si>
+  <si>
+    <t>SMD IC OP-AMP DUAL LM393AM</t>
   </si>
 </sst>
 </file>
@@ -965,8 +968,8 @@
   </sheetPr>
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -997,7 +1000,7 @@
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E3" s="11">
         <f>SUM(E5:E33)</f>
-        <v>50.907000000000004</v>
+        <v>34.007000000000005</v>
       </c>
       <c r="F3" s="12"/>
       <c r="G3" s="10"/>
@@ -1407,7 +1410,7 @@
         <v>13</v>
       </c>
       <c r="E27" s="13">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1421,10 +1424,10 @@
         <v>138</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>139</v>
+        <v>13</v>
       </c>
       <c r="E28" s="13">
-        <v>4</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="29" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1469,13 +1472,13 @@
         <v>146</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>148</v>
+        <v>174</v>
       </c>
       <c r="D31" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E31" s="13">
-        <v>15</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="32" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>